<commit_message>
numero da versao e pessoa para cliente
</commit_message>
<xml_diff>
--- a/modelo_op_carpintaria.xlsx
+++ b/modelo_op_carpintaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcp2\checklist_qualidade\qualidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88615D88-80A8-42F1-92BE-B4D883DFB6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D09994F-4B1C-45C0-BA15-1478BAB72F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>Código:</t>
   </si>
   <si>
-    <t>RQ CQ-011-000</t>
-  </si>
-  <si>
     <t>Data de Emissão:</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>DATA</t>
-  </si>
-  <si>
-    <t>PESSOA</t>
   </si>
   <si>
     <t>N° DE SÉRIE</t>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>QT</t>
+  </si>
+  <si>
+    <t>RQ CQ-011-002</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
   </si>
 </sst>
 </file>
@@ -694,6 +694,57 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -701,15 +752,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,48 +797,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6361,8 +6361,8 @@
   </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6381,265 +6381,265 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="60"/>
-      <c r="B1" s="62" t="s">
+      <c r="A1" s="50"/>
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="64" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="65"/>
+      <c r="G1" s="54"/>
       <c r="H1" s="18" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="64" t="s">
-        <v>4</v>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="43" t="s">
+        <v>3</v>
       </c>
-      <c r="G2" s="65"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="19">
         <v>44410</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="61"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="65"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="19">
         <v>45055</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="64" t="s">
-        <v>7</v>
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="43" t="s">
+        <v>6</v>
       </c>
-      <c r="G4" s="65"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="20">
         <v>44197</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="63" customHeight="1">
       <c r="A5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
+      <c r="K5" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="63"/>
+    </row>
+    <row r="6" spans="1:14" ht="103.5" customHeight="1">
+      <c r="A6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="15" t="s">
-        <v>29</v>
+      <c r="F6" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="E5" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
-      <c r="K5" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="49"/>
-    </row>
-    <row r="6" spans="1:14" ht="103.5" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="73"/>
       <c r="K6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="54" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="59"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
       <c r="K7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="81.75" customHeight="1">
       <c r="A8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="H8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>18</v>
-      </c>
       <c r="K8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="55.5" customHeight="1">
       <c r="A9" s="29"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="25"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="K9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="55.5" customHeight="1">
       <c r="A10" s="29"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="29"/>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
       <c r="K10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="55.5" customHeight="1">
       <c r="A11" s="29"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="29"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="K11" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="55.5" customHeight="1">
       <c r="A12" s="29"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="29"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="K12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="55.5" customHeight="1">
       <c r="A13" s="29"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="29"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="K13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L13" s="7"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" ht="55.5" customHeight="1" thickBot="1">
       <c r="A14" s="29"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="29"/>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="K14" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="55.5" customHeight="1" thickBot="1">
       <c r="A15" s="29"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="29"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="K15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="55.5" customHeight="1" thickBot="1">
       <c r="A16" s="29"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="29"/>
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="K16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="55.5" customHeight="1">
       <c r="A17" s="29"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="29"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
@@ -6647,9 +6647,9 @@
     </row>
     <row r="18" spans="1:8" ht="55.5" customHeight="1">
       <c r="A18" s="29"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="29"/>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
@@ -6657,9 +6657,9 @@
     </row>
     <row r="19" spans="1:8" ht="55.5" customHeight="1">
       <c r="A19" s="29"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="29"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
@@ -6667,9 +6667,9 @@
     </row>
     <row r="20" spans="1:8" ht="55.5" customHeight="1">
       <c r="A20" s="29"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="29"/>
       <c r="F20" s="27"/>
       <c r="G20" s="27"/>
@@ -6677,9 +6677,9 @@
     </row>
     <row r="21" spans="1:8" ht="55.5" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
       <c r="E21" s="29"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -6687,9 +6687,9 @@
     </row>
     <row r="22" spans="1:8" ht="55.5" customHeight="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="29"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
@@ -6697,9 +6697,9 @@
     </row>
     <row r="23" spans="1:8" ht="55.5" customHeight="1">
       <c r="A23" s="29"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="29"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
@@ -6707,9 +6707,9 @@
     </row>
     <row r="24" spans="1:8" ht="55.5" customHeight="1">
       <c r="A24" s="29"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
       <c r="E24" s="29"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
@@ -6717,9 +6717,9 @@
     </row>
     <row r="25" spans="1:8" ht="55.5" customHeight="1">
       <c r="A25" s="29"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="44"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="29"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
@@ -6727,9 +6727,9 @@
     </row>
     <row r="26" spans="1:8" ht="55.5" customHeight="1">
       <c r="A26" s="29"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="29"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -6737,9 +6737,9 @@
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" ht="55.5" customHeight="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="30"/>
       <c r="F27" s="26"/>
       <c r="G27" s="26"/>
@@ -6747,9 +6747,9 @@
     </row>
     <row r="28" spans="1:8" ht="55.5" customHeight="1">
       <c r="A28" s="29"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="29"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
@@ -6757,9 +6757,9 @@
     </row>
     <row r="29" spans="1:8" ht="55.5" customHeight="1">
       <c r="A29" s="29"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
       <c r="E29" s="29"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
@@ -6767,9 +6767,9 @@
     </row>
     <row r="30" spans="1:8" ht="55.5" customHeight="1">
       <c r="A30" s="29"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="29"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
@@ -6777,9 +6777,9 @@
     </row>
     <row r="31" spans="1:8" ht="55.5" customHeight="1">
       <c r="A31" s="29"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="29"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
@@ -6787,9 +6787,9 @@
     </row>
     <row r="32" spans="1:8" ht="55.5" customHeight="1">
       <c r="A32" s="29"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="29"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
@@ -6797,36 +6797,36 @@
     </row>
     <row r="33" spans="1:8" ht="55.5" customHeight="1">
       <c r="A33" s="29"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="41"/>
       <c r="E33" s="29"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="60" customHeight="1">
-      <c r="A34" s="72" t="s">
-        <v>19</v>
+      <c r="A34" s="48" t="s">
+        <v>17</v>
       </c>
-      <c r="B34" s="73"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="21" t="s">
+      <c r="G34" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="H34" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="54.95" customHeight="1">
@@ -6910,17 +6910,17 @@
       <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A43" s="67" t="s">
-        <v>22</v>
+      <c r="A43" s="42" t="s">
+        <v>20</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="70" t="s">
-        <v>23</v>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="46" t="s">
+        <v>21</v>
       </c>
-      <c r="G43" s="71"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="35"/>
     </row>
     <row r="44" spans="1:8" ht="20.25" thickTop="1">
@@ -6937,34 +6937,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
@@ -6981,6 +6953,34 @@
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
nova coluna e mudanca no cabeçalho
</commit_message>
<xml_diff>
--- a/modelo_op_carpintaria.xlsx
+++ b/modelo_op_carpintaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcp2\checklist_qualidade\qualidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF31282-C360-4E04-8FC5-585DA44E152E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C31FAF4-60CB-4AEE-86C6-D26BC20D7E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6391,8 +6391,8 @@
   </sheetPr>
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
mudanças de celulas e cabeçalho
</commit_message>
<xml_diff>
--- a/modelo_op_carpintaria.xlsx
+++ b/modelo_op_carpintaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcp2\checklist_qualidade\qualidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C31FAF4-60CB-4AEE-86C6-D26BC20D7E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59081A0-5CCB-4AA0-9F64-1B92E2B8337A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>CHECKLIST DA QUALIDADE</t>
   </si>
@@ -148,7 +145,7 @@
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="000000"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +320,13 @@
     <font>
       <sz val="22"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -603,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -637,9 +641,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,15 +710,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,21 +734,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -766,12 +743,27 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -811,6 +803,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,13 +821,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6392,7 +6393,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6411,571 +6412,569 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="60"/>
-      <c r="B1" s="62" t="s">
-        <v>35</v>
+      <c r="A1" s="56"/>
+      <c r="B1" s="58" t="s">
+        <v>34</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63" t="s">
-        <v>2</v>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="59" t="s">
+        <v>1</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="18" t="s">
-        <v>34</v>
+      <c r="G1" s="60"/>
+      <c r="H1" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="26.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63" t="s">
-        <v>3</v>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59" t="s">
+        <v>2</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="19">
+      <c r="G2" s="60"/>
+      <c r="H2" s="18">
         <v>45293</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="13" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="61"/>
-      <c r="B3" s="65" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="19" t="s">
-        <v>33</v>
+      <c r="G3" s="60"/>
+      <c r="H3" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="13" customFormat="1" ht="26.25">
-      <c r="A4" s="61"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="63" t="s">
-        <v>6</v>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="59" t="s">
+        <v>5</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="20">
+      <c r="G4" s="60"/>
+      <c r="H4" s="19">
         <v>44197</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="13" customFormat="1" ht="31.5">
-      <c r="A5" s="73" t="s">
-        <v>1</v>
+      <c r="A5" s="72" t="s">
+        <v>0</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="75"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="1:14" s="13" customFormat="1" ht="29.25" thickBot="1">
-      <c r="A6" s="76" t="s">
-        <v>36</v>
+      <c r="A6" s="69" t="s">
+        <v>35</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="78"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
     </row>
     <row r="7" spans="1:14" ht="63" customHeight="1">
       <c r="A7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="53"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="K7" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="45"/>
+    </row>
+    <row r="8" spans="1:14" ht="99.75" customHeight="1">
+      <c r="A8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="15" t="s">
-        <v>27</v>
+      <c r="F8" s="14" t="s">
+        <v>31</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="K7" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="49"/>
-    </row>
-    <row r="8" spans="1:14" ht="103.5" customHeight="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="58"/>
-      <c r="H8" s="59"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50"/>
       <c r="K8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="54" customHeight="1">
       <c r="A9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="59"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
       <c r="K9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="81.75" customHeight="1">
       <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>16</v>
-      </c>
       <c r="K10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A11" s="29"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="K11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
       <c r="K12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="K13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
       <c r="K14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
       <c r="K15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L15" s="7"/>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
       <c r="K16" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
       <c r="K17" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A18" s="29"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
       <c r="K18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A21" s="29"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A22" s="29"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A23" s="29"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A24" s="29"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A25" s="29"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A28" s="29"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:12" s="3" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A29" s="30"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
     </row>
     <row r="30" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:12" ht="55.5" customHeight="1">
-      <c r="A32" s="29"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:8" ht="55.5" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:8" ht="55.5" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" ht="55.5" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:8" ht="60" customHeight="1">
-      <c r="A36" s="71" t="s">
+      <c r="A36" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="68"/>
+      <c r="C36" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="11" t="s">
+      <c r="H36" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="36"/>
     </row>
     <row r="38" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36"/>
     </row>
     <row r="39" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36"/>
     </row>
     <row r="40" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
     </row>
     <row r="41" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
     </row>
     <row r="42" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="37"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="36"/>
     </row>
     <row r="43" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="36"/>
     </row>
     <row r="44" spans="1:8" ht="54.95" customHeight="1">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="37"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="36"/>
     </row>
     <row r="45" spans="1:8" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="59"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="63"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="70"/>
-      <c r="H45" s="35"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="34"/>
     </row>
     <row r="46" spans="1:8" ht="20.25" thickTop="1">
       <c r="A46" s="8"/>
@@ -6996,12 +6995,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F7:H7"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
@@ -7021,13 +7020,10 @@
     <mergeCell ref="B3:E4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A8:D8"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:H7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
@@ -7037,6 +7033,9 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>